<commit_message>
Added graphics t(N), n(N) and e(N)
</commit_message>
<xml_diff>
--- a/Homework1/stats.xlsx
+++ b/Homework1/stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.chernyakov\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.chernyakov\Desktop\BioAlg\Homework1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95B249C-153C-47BF-9B7D-7263D717C51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2A7AF0-7992-4DB8-8464-EEE5384099FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -74,9 +87,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -92,6 +104,3132 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>t(N)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$29:$J$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$30:$J$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-422B-4448-8402-3116BA3A4B87}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="372235936"/>
+        <c:axId val="372234496"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="372235936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Мощность популяции</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="372234496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="372234496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Время работы алгоритма</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="372235936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>n(N)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$29:$J$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$31:$J$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>35.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F798-4044-B3C6-0BF701BEA26B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="497446096"/>
+        <c:axId val="497444656"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="497446096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Мощность популяции</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="497444656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="497444656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Число</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> поколений</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="497446096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>e(N)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$29:$J$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$32:$J$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>52.785581258968683</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.733405835000013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.952177051000014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52.914605492999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.07610491799997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52.953396158999986</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52.914370762999937</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52.914370766999987</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8E38-469D-B198-5D31849611FE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="684317472"/>
+        <c:axId val="684315672"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="684317472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Мощность</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> популяции</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="684315672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="684315672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Точность решения</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="684317472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Диаграмма 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{822D3D80-E4D4-9AE8-B519-E3CB5740CE09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Диаграмма 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{098B945F-F2F9-D688-27AA-9AA1D34C7085}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Диаграмма 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18534106-9A91-1786-B874-826E3976D594}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -359,8 +3497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:X32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="Z38" sqref="Z38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +4042,7 @@
         <v>2.5270135847400002</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="D14:X14" si="0">SUM(F16:F25)/10</f>
+        <f t="shared" ref="F14:X14" si="0">SUM(F16:F25)/10</f>
         <v>2.5273340583500001</v>
       </c>
       <c r="I14">
@@ -936,12 +4074,10 @@
       <c r="B16">
         <v>2.5291437000000001</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>2.5291437075999998</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
+      <c r="F16">
         <v>2.5291437073999998</v>
       </c>
       <c r="I16">
@@ -963,13 +4099,11 @@
         <v>2.5291437083999999</v>
       </c>
     </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C17" s="1">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C17">
         <v>2.5291437072999998</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>2.5205975264</v>
       </c>
       <c r="I17">
@@ -991,13 +4125,11 @@
         <v>2.5291437078999999</v>
       </c>
     </row>
-    <row r="18" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C18" s="1">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C18">
         <v>2.5291437081999999</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1">
+      <c r="F18">
         <v>2.5291437074999998</v>
       </c>
       <c r="I18">
@@ -1019,13 +4151,11 @@
         <v>2.5291437082999999</v>
       </c>
     </row>
-    <row r="19" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C19" s="1">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C19">
         <v>2.5291437076999999</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>2.5192334579</v>
       </c>
       <c r="I19">
@@ -1047,13 +4177,11 @@
         <v>2.5291437077999999</v>
       </c>
     </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C20" s="1">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C20">
         <v>2.5291437076999999</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1">
+      <c r="F20">
         <v>2.5291437092</v>
       </c>
       <c r="I20">
@@ -1075,13 +4203,11 @@
         <v>2.5291437072999998</v>
       </c>
     </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C21" s="1">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C21">
         <v>2.5291436989</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1">
+      <c r="F21">
         <v>2.5290725153000002</v>
       </c>
       <c r="I21">
@@ -1103,13 +4229,11 @@
         <v>2.5291437069999998</v>
       </c>
     </row>
-    <row r="22" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C22" s="1">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C22">
         <v>2.5291438014000001</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1">
+      <c r="F22">
         <v>2.5295749716999998</v>
       </c>
       <c r="I22">
@@ -1131,13 +4255,11 @@
         <v>2.5291437070999998</v>
       </c>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C23" s="1">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C23">
         <v>2.5363433722000002</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1">
+      <c r="F23">
         <v>2.5291437128999998</v>
       </c>
       <c r="I23">
@@ -1159,13 +4281,11 @@
         <v>2.5291437080999999</v>
       </c>
     </row>
-    <row r="24" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C24" s="1">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C24">
         <v>2.5006427286999999</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1">
+      <c r="F24">
         <v>2.5291437074999998</v>
       </c>
       <c r="I24">
@@ -1187,13 +4307,11 @@
         <v>2.5291437073999998</v>
       </c>
     </row>
-    <row r="25" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C25" s="1">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C25">
         <v>2.5291437076999999</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1">
+      <c r="F25">
         <v>2.5291435676999998</v>
       </c>
       <c r="I25">
@@ -1215,13 +4333,16 @@
         <v>2.5291437073999998</v>
       </c>
     </row>
-    <row r="26" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C26">
         <f>COUNT(C16:C25)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>0</v>
+      </c>
       <c r="C29">
         <v>30</v>
       </c>
@@ -1247,7 +4368,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
       <c r="C30">
         <f>SUM(B3:B12)/10</f>
         <v>5.3</v>
@@ -1281,7 +4405,10 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="31" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
       <c r="C31">
         <f>SUM(C3:C12)/10</f>
         <v>35.5</v>
@@ -1315,7 +4442,10 @@
         <v>41.8</v>
       </c>
     </row>
-    <row r="32" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
       <c r="C32">
         <f>ABS(1-(C14-C14/B14))*100</f>
         <v>52.785581258968683</v>
@@ -1353,6 +4483,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">

</xml_diff>